<commit_message>
GITBOOK-169: change request with no subject merged in GitBook
</commit_message>
<xml_diff>
--- a/.gitbook/assets/example 2.xlsx
+++ b/.gitbook/assets/example 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64145A2-C3B8-4B67-A9DD-8FC02A97DC42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B681D8-5E80-4889-ACF6-4F4893783D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5730" yWindow="780" windowWidth="19290" windowHeight="9765" xr2:uid="{E93A209E-A357-4852-8FEC-CD32255DCE1F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E93A209E-A357-4852-8FEC-CD32255DCE1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>email1@gmail.com</t>
   </si>
@@ -85,6 +85,45 @@
   </si>
   <si>
     <t>pass10</t>
+  </si>
+  <si>
+    <t>9a757855-def8-4ffe-b2f7-882be9bada10</t>
+  </si>
+  <si>
+    <t>9a735c1d-0131-4387-a82b-76ef177630d3</t>
+  </si>
+  <si>
+    <t>9a735c1c-9c34-428a-bae3-acc6f1b094e8</t>
+  </si>
+  <si>
+    <t>9a735c1c-4a50-4be1-a458-e22e360b165f</t>
+  </si>
+  <si>
+    <t>9a735c1b-ebc4-4f7d-88cf-ca6796736b82</t>
+  </si>
+  <si>
+    <t>9a735c1b-8e72-417f-875d-c3a59ddba5e2</t>
+  </si>
+  <si>
+    <t>9a735c1b-37ee-4484-829d-f23803e1ccf0</t>
+  </si>
+  <si>
+    <t>9a735c1a-d66a-4b34-b6c7-26983f935ea5</t>
+  </si>
+  <si>
+    <t>9a735c1a-7714-42e1-a937-6540b962d3f0</t>
+  </si>
+  <si>
+    <t>9a735c1a-182e-45b5-8041-3b9dee4e5b92</t>
+  </si>
+  <si>
+    <t>uuid</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>pass</t>
   </si>
 </sst>
 </file>
@@ -436,95 +475,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECAD758C-DF4A-49E5-930E-3DE894AE4200}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="41.140625" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C11" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>